<commit_message>
Implement cascading product search for cost importer
- Update cost_importer.py with cascading search logic:
  * Search by SKU (sku_ozon) first - priority method
  * Fallback to barcode search if not found by SKU
  * Enhanced logging shows which field matched

- Change Excel format from 'barcode' to 'product_id':
  * Single column accepts both SKU and barcode values
  * Automatic detection and cascading search
  * Simplified user experience

- Update test files with new format:
  * Mixed test data with SKUs and barcodes
  * Updated test_cost_importer.py logic

- Update documentation:
  * Explain cascading search behavior
  * New Excel format examples
  * Updated SQL queries for verification

System now provides maximum product coverage with reliable SKU priority
</commit_message>
<xml_diff>
--- a/uploads/cost_price.xlsx
+++ b/uploads/cost_price.xlsx
@@ -16,25 +16,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>barcode</t>
+    <t>product_id</t>
   </si>
   <si>
     <t>cost_price</t>
   </si>
   <si>
-    <t>4607034370237</t>
+    <t>SKU123456</t>
   </si>
   <si>
     <t>4607034370244</t>
   </si>
   <si>
-    <t>4607034370251</t>
+    <t>OZON789012</t>
   </si>
   <si>
     <t>9999999999999</t>
   </si>
   <si>
-    <t>1111111111111</t>
+    <t>UNKNOWN_SKU</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Adapt cost importer to Russian column names
- Update EXPECTED_COLUMNS to match real Excel format:
  * 'баркод' (barcode)
  * 'артикул' (article/SKU)
  * 'СС без НДС' (cost price without VAT)

- Improve validation logic:
  * Requires 'СС без НДС' column (mandatory)
  * Requires either 'баркод' OR 'артикул' (flexible)
  * Better error messages for missing columns

- Update cascading search logic:
  * Search by 'артикул' → sku_ozon in database
  * Fallback to 'баркод' → barcode in database
  * Enhanced logging shows which field matched

- Create test file with Russian columns matching real data format

System now works with actual client Excel files with Russian headers
</commit_message>
<xml_diff>
--- a/uploads/cost_price.xlsx
+++ b/uploads/cost_price.xlsx
@@ -14,27 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>product_id</t>
-  </si>
-  <si>
-    <t>cost_price</t>
-  </si>
-  <si>
-    <t>SKU123456</t>
-  </si>
-  <si>
-    <t>4607034370244</t>
-  </si>
-  <si>
-    <t>OZON789012</t>
-  </si>
-  <si>
-    <t>9999999999999</t>
-  </si>
-  <si>
-    <t>UNKNOWN_SKU</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>баркод</t>
+  </si>
+  <si>
+    <t>артикул</t>
+  </si>
+  <si>
+    <t>СС с НДС</t>
+  </si>
+  <si>
+    <t>СС без НДС</t>
+  </si>
+  <si>
+    <t>4600956001999</t>
+  </si>
+  <si>
+    <t>4600956006390</t>
+  </si>
+  <si>
+    <t>4600956009759</t>
+  </si>
+  <si>
+    <t>4600956001777</t>
+  </si>
+  <si>
+    <t>4600956002040</t>
+  </si>
+  <si>
+    <t>Хлопья_арахис 250г</t>
+  </si>
+  <si>
+    <t>Ассорти3,0</t>
+  </si>
+  <si>
+    <t>Ирис_молочн_байтс500г</t>
+  </si>
+  <si>
+    <t>Хлопья_мед 300г</t>
+  </si>
+  <si>
+    <t>Конфеты_микс_лимт 100г</t>
   </si>
 </sst>
 </file>
@@ -392,58 +413,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>150.5</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>92.983</v>
+      </c>
+      <c r="D2">
+        <v>84.53</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1071.18</v>
+      </c>
+      <c r="D3">
+        <v>892.65</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>175.25</v>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>186.696</v>
+      </c>
+      <c r="D4">
+        <v>155.58</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>300.75</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>83.688</v>
+      </c>
+      <c r="D5">
+        <v>76.08</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>125</v>
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>187.668</v>
+      </c>
+      <c r="D6">
+        <v>156.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>